<commit_message>
added gitignore, codebase etc
</commit_message>
<xml_diff>
--- a/Dokumente/Planen/00_Projektablauf_Gantt.xlsx
+++ b/Dokumente/Planen/00_Projektablauf_Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvesj\source\2025_TerminalChat\Dokumente\Planen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvesj\source\ims.project.terminalchat\Dokumente\Planen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F2B38-D812-4DA0-BE93-1C120A197966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75BA71-AB1F-417A-B421-6EC5EA778A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27795" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -891,6 +891,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -908,12 +914,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,26 +1202,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP4" sqref="AP4:AP51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="13" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="51" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="13" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="51" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:52" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:52" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>100</v>
       </c>
@@ -1234,16 +1234,16 @@
       <c r="O2" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="U2" s="54" t="s">
+      <c r="U2" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-    </row>
-    <row r="3" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+    </row>
+    <row r="3" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
         <v>0</v>
       </c>
@@ -1325,52 +1325,52 @@
       <c r="AA3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AB3" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AC3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AE3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AF3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AG3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AH3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AI3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AJ3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AK3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AL3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AM3" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AN3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AO3" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AP3" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AQ3" s="30" t="s">
         <v>43</v>
       </c>
       <c r="AR3" s="8" t="s">
@@ -1401,7 +1401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>90</v>
       </c>
@@ -1433,33 +1433,33 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
       <c r="AC4" s="20"/>
-      <c r="AD4" s="47"/>
+      <c r="AD4" s="49"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="20"/>
       <c r="AG4" s="20"/>
       <c r="AH4" s="20"/>
       <c r="AI4" s="20"/>
-      <c r="AJ4" s="47"/>
+      <c r="AJ4" s="49"/>
       <c r="AK4" s="20"/>
       <c r="AL4" s="20"/>
       <c r="AM4" s="20"/>
       <c r="AN4" s="20"/>
       <c r="AO4" s="20"/>
-      <c r="AP4" s="47"/>
+      <c r="AP4" s="49"/>
       <c r="AQ4" s="20"/>
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
       <c r="AT4" s="20"/>
       <c r="AU4" s="20"/>
-      <c r="AV4" s="47"/>
+      <c r="AV4" s="49"/>
       <c r="AW4" s="20"/>
       <c r="AX4" s="20"/>
       <c r="AY4" s="20"/>
-      <c r="AZ4" s="50" t="s">
+      <c r="AZ4" s="52" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>53</v>
       </c>
@@ -1497,31 +1497,31 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="48"/>
+      <c r="AD5" s="50"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="48"/>
+      <c r="AJ5" s="50"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
-      <c r="AP5" s="48"/>
+      <c r="AP5" s="50"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
-      <c r="AV5" s="48"/>
+      <c r="AV5" s="50"/>
       <c r="AW5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
-      <c r="AZ5" s="51"/>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ5" s="53"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>53</v>
       </c>
@@ -1557,31 +1557,31 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="48"/>
+      <c r="AD6" s="50"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="48"/>
+      <c r="AJ6" s="50"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="48"/>
+      <c r="AP6" s="50"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
-      <c r="AV6" s="48"/>
+      <c r="AV6" s="50"/>
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
-      <c r="AZ6" s="51"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ6" s="53"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>53</v>
       </c>
@@ -1617,31 +1617,31 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="48"/>
+      <c r="AD7" s="50"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="48"/>
+      <c r="AJ7" s="50"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="48"/>
+      <c r="AP7" s="50"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
-      <c r="AV7" s="48"/>
+      <c r="AV7" s="50"/>
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
-      <c r="AZ7" s="51"/>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ7" s="53"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>53</v>
       </c>
@@ -1677,31 +1677,31 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="48"/>
+      <c r="AD8" s="50"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
-      <c r="AJ8" s="48"/>
+      <c r="AJ8" s="50"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
-      <c r="AP8" s="48"/>
+      <c r="AP8" s="50"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
-      <c r="AV8" s="48"/>
+      <c r="AV8" s="50"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
-      <c r="AZ8" s="51"/>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ8" s="53"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>53</v>
       </c>
@@ -1737,31 +1737,31 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="48"/>
+      <c r="AD9" s="50"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="48"/>
+      <c r="AJ9" s="50"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
-      <c r="AP9" s="48"/>
+      <c r="AP9" s="50"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
       <c r="AS9" s="2"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
-      <c r="AV9" s="48"/>
+      <c r="AV9" s="50"/>
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
-      <c r="AZ9" s="51"/>
-    </row>
-    <row r="10" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AZ9" s="53"/>
+    </row>
+    <row r="10" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
         <v>53</v>
       </c>
@@ -1799,31 +1799,31 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="48"/>
+      <c r="AD10" s="50"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-      <c r="AJ10" s="48"/>
+      <c r="AJ10" s="50"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
-      <c r="AP10" s="48"/>
+      <c r="AP10" s="50"/>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2"/>
       <c r="AS10" s="2"/>
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
-      <c r="AV10" s="48"/>
+      <c r="AV10" s="50"/>
       <c r="AW10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
-      <c r="AZ10" s="51"/>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ10" s="53"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>53</v>
       </c>
@@ -1859,31 +1859,31 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="48"/>
+      <c r="AD11" s="50"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
-      <c r="AJ11" s="48"/>
+      <c r="AJ11" s="50"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
-      <c r="AP11" s="48"/>
+      <c r="AP11" s="50"/>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
-      <c r="AV11" s="48"/>
+      <c r="AV11" s="50"/>
       <c r="AW11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
-      <c r="AZ11" s="51"/>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ11" s="53"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>53</v>
       </c>
@@ -1919,31 +1919,31 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="48"/>
+      <c r="AD12" s="50"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="48"/>
+      <c r="AJ12" s="50"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
-      <c r="AP12" s="48"/>
+      <c r="AP12" s="50"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
       <c r="AS12" s="2"/>
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
-      <c r="AV12" s="48"/>
+      <c r="AV12" s="50"/>
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
-      <c r="AZ12" s="51"/>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ12" s="53"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>53</v>
       </c>
@@ -1979,31 +1979,31 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="48"/>
+      <c r="AD13" s="50"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="48"/>
+      <c r="AJ13" s="50"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
-      <c r="AP13" s="48"/>
+      <c r="AP13" s="50"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
       <c r="AS13" s="2"/>
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
-      <c r="AV13" s="48"/>
+      <c r="AV13" s="50"/>
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
-      <c r="AZ13" s="51"/>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ13" s="53"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>53</v>
       </c>
@@ -2039,31 +2039,31 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="48"/>
+      <c r="AD14" s="50"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-      <c r="AJ14" s="48"/>
+      <c r="AJ14" s="50"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
-      <c r="AP14" s="48"/>
+      <c r="AP14" s="50"/>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="2"/>
       <c r="AU14" s="2"/>
-      <c r="AV14" s="48"/>
+      <c r="AV14" s="50"/>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
-      <c r="AZ14" s="51"/>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ14" s="53"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>53</v>
       </c>
@@ -2099,31 +2099,31 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="48"/>
+      <c r="AD15" s="50"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="48"/>
+      <c r="AJ15" s="50"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
-      <c r="AP15" s="48"/>
+      <c r="AP15" s="50"/>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2"/>
       <c r="AS15" s="2"/>
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
-      <c r="AV15" s="48"/>
+      <c r="AV15" s="50"/>
       <c r="AW15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
-      <c r="AZ15" s="51"/>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ15" s="53"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>53</v>
       </c>
@@ -2157,31 +2157,31 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="48"/>
+      <c r="AD16" s="50"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
-      <c r="AJ16" s="48"/>
+      <c r="AJ16" s="50"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="48"/>
+      <c r="AP16" s="50"/>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
-      <c r="AV16" s="48"/>
+      <c r="AV16" s="50"/>
       <c r="AW16" s="2"/>
       <c r="AX16" s="2"/>
       <c r="AY16" s="2"/>
-      <c r="AZ16" s="51"/>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ16" s="53"/>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>53</v>
       </c>
@@ -2217,31 +2217,31 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="48"/>
+      <c r="AD17" s="50"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="48"/>
+      <c r="AJ17" s="50"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="48"/>
+      <c r="AP17" s="50"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
       <c r="AS17" s="2"/>
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
-      <c r="AV17" s="48"/>
+      <c r="AV17" s="50"/>
       <c r="AW17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
-      <c r="AZ17" s="51"/>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ17" s="53"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>53</v>
       </c>
@@ -2277,31 +2277,31 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
-      <c r="AD18" s="48"/>
+      <c r="AD18" s="50"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="48"/>
+      <c r="AJ18" s="50"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
-      <c r="AP18" s="48"/>
+      <c r="AP18" s="50"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
       <c r="AS18" s="2"/>
       <c r="AT18" s="2"/>
       <c r="AU18" s="2"/>
-      <c r="AV18" s="48"/>
+      <c r="AV18" s="50"/>
       <c r="AW18" s="2"/>
       <c r="AX18" s="2"/>
       <c r="AY18" s="2"/>
-      <c r="AZ18" s="51"/>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ18" s="53"/>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>53</v>
       </c>
@@ -2343,31 +2343,31 @@
       <c r="AC19" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="AD19" s="48"/>
+      <c r="AD19" s="50"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-      <c r="AJ19" s="48"/>
+      <c r="AJ19" s="50"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
-      <c r="AP19" s="48"/>
+      <c r="AP19" s="50"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
       <c r="AS19" s="2"/>
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
-      <c r="AV19" s="48"/>
+      <c r="AV19" s="50"/>
       <c r="AW19" s="2"/>
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
-      <c r="AZ19" s="51"/>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ19" s="53"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
         <v>89</v>
       </c>
@@ -2399,31 +2399,31 @@
       <c r="AA20" s="24"/>
       <c r="AB20" s="24"/>
       <c r="AC20" s="24"/>
-      <c r="AD20" s="48"/>
+      <c r="AD20" s="50"/>
       <c r="AE20" s="24"/>
       <c r="AF20" s="24"/>
       <c r="AG20" s="24"/>
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
-      <c r="AJ20" s="48"/>
+      <c r="AJ20" s="50"/>
       <c r="AK20" s="24"/>
       <c r="AL20" s="24"/>
       <c r="AM20" s="24"/>
       <c r="AN20" s="24"/>
       <c r="AO20" s="24"/>
-      <c r="AP20" s="48"/>
+      <c r="AP20" s="50"/>
       <c r="AQ20" s="24"/>
       <c r="AR20" s="24"/>
       <c r="AS20" s="24"/>
       <c r="AT20" s="24"/>
       <c r="AU20" s="24"/>
-      <c r="AV20" s="48"/>
+      <c r="AV20" s="50"/>
       <c r="AW20" s="24"/>
       <c r="AX20" s="24"/>
       <c r="AY20" s="24"/>
-      <c r="AZ20" s="51"/>
-    </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ20" s="53"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>62</v>
       </c>
@@ -2455,33 +2455,33 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
-      <c r="AB21" s="53"/>
+      <c r="AB21" s="47"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="48"/>
+      <c r="AD21" s="50"/>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="48"/>
+      <c r="AJ21" s="50"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
-      <c r="AP21" s="48"/>
+      <c r="AP21" s="50"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
-      <c r="AV21" s="48"/>
+      <c r="AV21" s="50"/>
       <c r="AW21" s="2"/>
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
-      <c r="AZ21" s="51"/>
-    </row>
-    <row r="22" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AZ21" s="53"/>
+    </row>
+    <row r="22" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>62</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>105</v>
       </c>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="48"/>
+      <c r="AD22" s="50"/>
       <c r="AE22" s="44" t="s">
         <v>106</v>
       </c>
@@ -2527,25 +2527,25 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
-      <c r="AJ22" s="48"/>
+      <c r="AJ22" s="50"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
-      <c r="AP22" s="48"/>
+      <c r="AP22" s="50"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
       <c r="AS22" s="2"/>
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
-      <c r="AV22" s="48"/>
+      <c r="AV22" s="50"/>
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
-      <c r="AZ22" s="51"/>
-    </row>
-    <row r="23" spans="1:52" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AZ22" s="53"/>
+    </row>
+    <row r="23" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>62</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="48"/>
+      <c r="AD23" s="50"/>
       <c r="AE23" s="44" t="s">
         <v>106</v>
       </c>
@@ -2589,25 +2589,25 @@
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="48"/>
+      <c r="AJ23" s="50"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="48"/>
+      <c r="AP23" s="50"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
-      <c r="AV23" s="48"/>
+      <c r="AV23" s="50"/>
       <c r="AW23" s="2"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
-      <c r="AZ23" s="51"/>
-    </row>
-    <row r="24" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AZ23" s="53"/>
+    </row>
+    <row r="24" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>62</v>
       </c>
@@ -2643,7 +2643,7 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="48"/>
+      <c r="AD24" s="50"/>
       <c r="AE24" s="2"/>
       <c r="AF24" s="44" t="s">
         <v>106</v>
@@ -2651,25 +2651,25 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-      <c r="AJ24" s="48"/>
+      <c r="AJ24" s="50"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
-      <c r="AP24" s="48"/>
+      <c r="AP24" s="50"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
       <c r="AS24" s="2"/>
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
-      <c r="AV24" s="48"/>
+      <c r="AV24" s="50"/>
       <c r="AW24" s="2"/>
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
-      <c r="AZ24" s="51"/>
-    </row>
-    <row r="25" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AZ24" s="53"/>
+    </row>
+    <row r="25" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>62</v>
       </c>
@@ -2705,7 +2705,7 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="48"/>
+      <c r="AD25" s="50"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="44" t="s">
         <v>106</v>
@@ -2713,25 +2713,25 @@
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="48"/>
+      <c r="AJ25" s="50"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
-      <c r="AP25" s="48"/>
+      <c r="AP25" s="50"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
       <c r="AS25" s="2"/>
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
-      <c r="AV25" s="48"/>
+      <c r="AV25" s="50"/>
       <c r="AW25" s="2"/>
       <c r="AX25" s="2"/>
       <c r="AY25" s="2"/>
-      <c r="AZ25" s="51"/>
-    </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ25" s="53"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>62</v>
       </c>
@@ -2765,31 +2765,31 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="48"/>
+      <c r="AD26" s="50"/>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="48"/>
+      <c r="AJ26" s="50"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
-      <c r="AP26" s="48"/>
+      <c r="AP26" s="50"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
-      <c r="AV26" s="48"/>
+      <c r="AV26" s="50"/>
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
-      <c r="AZ26" s="51"/>
-    </row>
-    <row r="27" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AZ26" s="53"/>
+    </row>
+    <row r="27" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
         <v>62</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
-      <c r="AD27" s="48"/>
+      <c r="AD27" s="50"/>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="44" t="s">
@@ -2833,25 +2833,25 @@
       </c>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
-      <c r="AJ27" s="48"/>
+      <c r="AJ27" s="50"/>
       <c r="AK27" s="2"/>
       <c r="AL27" s="2"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
-      <c r="AP27" s="48"/>
+      <c r="AP27" s="50"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
       <c r="AS27" s="2"/>
       <c r="AT27" s="2"/>
       <c r="AU27" s="2"/>
-      <c r="AV27" s="48"/>
+      <c r="AV27" s="50"/>
       <c r="AW27" s="2"/>
       <c r="AX27" s="2"/>
       <c r="AY27" s="2"/>
-      <c r="AZ27" s="51"/>
-    </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ27" s="53"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
         <v>62</v>
       </c>
@@ -2885,31 +2885,31 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-      <c r="AD28" s="48"/>
+      <c r="AD28" s="50"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-      <c r="AJ28" s="48"/>
+      <c r="AJ28" s="50"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
-      <c r="AP28" s="48"/>
+      <c r="AP28" s="50"/>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
       <c r="AS28" s="2"/>
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
-      <c r="AV28" s="48"/>
+      <c r="AV28" s="50"/>
       <c r="AW28" s="2"/>
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
-      <c r="AZ28" s="51"/>
-    </row>
-    <row r="29" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AZ28" s="53"/>
+    </row>
+    <row r="29" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
         <v>62</v>
       </c>
@@ -2945,7 +2945,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="48"/>
+      <c r="AD29" s="50"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
@@ -2953,25 +2953,25 @@
         <v>106</v>
       </c>
       <c r="AI29" s="2"/>
-      <c r="AJ29" s="48"/>
+      <c r="AJ29" s="50"/>
       <c r="AK29" s="2"/>
       <c r="AL29" s="2"/>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
-      <c r="AP29" s="48"/>
+      <c r="AP29" s="50"/>
       <c r="AQ29" s="2"/>
       <c r="AR29" s="2"/>
       <c r="AS29" s="2"/>
       <c r="AT29" s="2"/>
       <c r="AU29" s="2"/>
-      <c r="AV29" s="48"/>
+      <c r="AV29" s="50"/>
       <c r="AW29" s="2"/>
       <c r="AX29" s="2"/>
       <c r="AY29" s="2"/>
-      <c r="AZ29" s="51"/>
-    </row>
-    <row r="30" spans="1:52" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AZ29" s="53"/>
+    </row>
+    <row r="30" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
         <v>62</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-      <c r="AD30" s="48"/>
+      <c r="AD30" s="50"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
@@ -3015,25 +3015,25 @@
         <v>106</v>
       </c>
       <c r="AI30" s="2"/>
-      <c r="AJ30" s="48"/>
+      <c r="AJ30" s="50"/>
       <c r="AK30" s="2"/>
       <c r="AL30" s="2"/>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
-      <c r="AP30" s="48"/>
+      <c r="AP30" s="50"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="2"/>
       <c r="AS30" s="2"/>
       <c r="AT30" s="2"/>
       <c r="AU30" s="2"/>
-      <c r="AV30" s="48"/>
+      <c r="AV30" s="50"/>
       <c r="AW30" s="2"/>
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
-      <c r="AZ30" s="51"/>
-    </row>
-    <row r="31" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AZ30" s="53"/>
+    </row>
+    <row r="31" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>62</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="48"/>
+      <c r="AD31" s="50"/>
       <c r="AE31" s="2"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
@@ -3077,25 +3077,25 @@
       <c r="AI31" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AJ31" s="48"/>
+      <c r="AJ31" s="50"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="2"/>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
       <c r="AO31" s="2"/>
-      <c r="AP31" s="48"/>
+      <c r="AP31" s="50"/>
       <c r="AQ31" s="2"/>
       <c r="AR31" s="2"/>
       <c r="AS31" s="2"/>
       <c r="AT31" s="2"/>
       <c r="AU31" s="2"/>
-      <c r="AV31" s="48"/>
+      <c r="AV31" s="50"/>
       <c r="AW31" s="2"/>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
-      <c r="AZ31" s="51"/>
-    </row>
-    <row r="32" spans="1:52" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="AZ31" s="53"/>
+    </row>
+    <row r="32" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>62</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="48"/>
+      <c r="AD32" s="50"/>
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
@@ -3139,25 +3139,25 @@
       <c r="AI32" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AJ32" s="48"/>
+      <c r="AJ32" s="50"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
-      <c r="AP32" s="48"/>
+      <c r="AP32" s="50"/>
       <c r="AQ32" s="2"/>
       <c r="AR32" s="2"/>
       <c r="AS32" s="2"/>
       <c r="AT32" s="2"/>
       <c r="AU32" s="2"/>
-      <c r="AV32" s="48"/>
+      <c r="AV32" s="50"/>
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
-      <c r="AZ32" s="51"/>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ32" s="53"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>88</v>
       </c>
@@ -3189,31 +3189,31 @@
       <c r="AA33" s="24"/>
       <c r="AB33" s="24"/>
       <c r="AC33" s="24"/>
-      <c r="AD33" s="48"/>
+      <c r="AD33" s="50"/>
       <c r="AE33" s="24"/>
       <c r="AF33" s="24"/>
       <c r="AG33" s="24"/>
       <c r="AH33" s="24"/>
       <c r="AI33" s="24"/>
-      <c r="AJ33" s="48"/>
+      <c r="AJ33" s="50"/>
       <c r="AK33" s="24"/>
       <c r="AL33" s="24"/>
       <c r="AM33" s="24"/>
       <c r="AN33" s="24"/>
       <c r="AO33" s="24"/>
-      <c r="AP33" s="48"/>
+      <c r="AP33" s="50"/>
       <c r="AQ33" s="24"/>
       <c r="AR33" s="24"/>
       <c r="AS33" s="24"/>
       <c r="AT33" s="24"/>
       <c r="AU33" s="24"/>
-      <c r="AV33" s="48"/>
+      <c r="AV33" s="50"/>
       <c r="AW33" s="24"/>
       <c r="AX33" s="24"/>
       <c r="AY33" s="24"/>
-      <c r="AZ33" s="51"/>
-    </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ33" s="53"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>79</v>
       </c>
@@ -3247,13 +3247,13 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="48"/>
+      <c r="AD34" s="50"/>
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="48"/>
+      <c r="AJ34" s="50"/>
       <c r="AK34" s="44" t="s">
         <v>106</v>
       </c>
@@ -3261,19 +3261,19 @@
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2"/>
-      <c r="AP34" s="48"/>
+      <c r="AP34" s="50"/>
       <c r="AQ34" s="2"/>
       <c r="AR34" s="2"/>
       <c r="AS34" s="2"/>
       <c r="AT34" s="2"/>
       <c r="AU34" s="2"/>
-      <c r="AV34" s="48"/>
+      <c r="AV34" s="50"/>
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
-      <c r="AZ34" s="51"/>
-    </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ34" s="53"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>79</v>
       </c>
@@ -3307,13 +3307,13 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
-      <c r="AD35" s="48"/>
+      <c r="AD35" s="50"/>
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-      <c r="AJ35" s="48"/>
+      <c r="AJ35" s="50"/>
       <c r="AK35" s="44" t="s">
         <v>106</v>
       </c>
@@ -3321,19 +3321,19 @@
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
       <c r="AO35" s="2"/>
-      <c r="AP35" s="48"/>
+      <c r="AP35" s="50"/>
       <c r="AQ35" s="2"/>
       <c r="AR35" s="2"/>
       <c r="AS35" s="2"/>
       <c r="AT35" s="2"/>
       <c r="AU35" s="2"/>
-      <c r="AV35" s="48"/>
+      <c r="AV35" s="50"/>
       <c r="AW35" s="2"/>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
-      <c r="AZ35" s="51"/>
-    </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ35" s="53"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>79</v>
       </c>
@@ -3367,13 +3367,13 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="48"/>
+      <c r="AD36" s="50"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-      <c r="AJ36" s="48"/>
+      <c r="AJ36" s="50"/>
       <c r="AK36" s="44" t="s">
         <v>106</v>
       </c>
@@ -3381,19 +3381,19 @@
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
-      <c r="AP36" s="48"/>
+      <c r="AP36" s="50"/>
       <c r="AQ36" s="2"/>
       <c r="AR36" s="2"/>
       <c r="AS36" s="2"/>
       <c r="AT36" s="2"/>
       <c r="AU36" s="2"/>
-      <c r="AV36" s="48"/>
+      <c r="AV36" s="50"/>
       <c r="AW36" s="2"/>
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
-      <c r="AZ36" s="51"/>
-    </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ36" s="53"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>79</v>
       </c>
@@ -3427,13 +3427,13 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-      <c r="AD37" s="48"/>
+      <c r="AD37" s="50"/>
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-      <c r="AJ37" s="48"/>
+      <c r="AJ37" s="50"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="44" t="s">
         <v>106</v>
@@ -3441,19 +3441,19 @@
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
-      <c r="AP37" s="48"/>
+      <c r="AP37" s="50"/>
       <c r="AQ37" s="2"/>
       <c r="AR37" s="2"/>
       <c r="AS37" s="2"/>
       <c r="AT37" s="2"/>
       <c r="AU37" s="2"/>
-      <c r="AV37" s="48"/>
+      <c r="AV37" s="50"/>
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
-      <c r="AZ37" s="51"/>
-    </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ37" s="53"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>79</v>
       </c>
@@ -3487,13 +3487,13 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="48"/>
+      <c r="AD38" s="50"/>
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
-      <c r="AJ38" s="48"/>
+      <c r="AJ38" s="50"/>
       <c r="AK38" s="2"/>
       <c r="AL38" s="44" t="s">
         <v>106</v>
@@ -3501,19 +3501,19 @@
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
       <c r="AO38" s="2"/>
-      <c r="AP38" s="48"/>
+      <c r="AP38" s="50"/>
       <c r="AQ38" s="2"/>
       <c r="AR38" s="2"/>
       <c r="AS38" s="2"/>
       <c r="AT38" s="2"/>
       <c r="AU38" s="2"/>
-      <c r="AV38" s="48"/>
+      <c r="AV38" s="50"/>
       <c r="AW38" s="2"/>
       <c r="AX38" s="2"/>
       <c r="AY38" s="2"/>
-      <c r="AZ38" s="51"/>
-    </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ38" s="53"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
         <v>79</v>
       </c>
@@ -3547,13 +3547,13 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="48"/>
+      <c r="AD39" s="50"/>
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
-      <c r="AJ39" s="48"/>
+      <c r="AJ39" s="50"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="2"/>
       <c r="AM39" s="44" t="s">
@@ -3561,19 +3561,19 @@
       </c>
       <c r="AN39" s="2"/>
       <c r="AO39" s="2"/>
-      <c r="AP39" s="48"/>
+      <c r="AP39" s="50"/>
       <c r="AQ39" s="2"/>
       <c r="AR39" s="2"/>
       <c r="AS39" s="2"/>
       <c r="AT39" s="2"/>
       <c r="AU39" s="2"/>
-      <c r="AV39" s="48"/>
+      <c r="AV39" s="50"/>
       <c r="AW39" s="2"/>
       <c r="AX39" s="2"/>
       <c r="AY39" s="2"/>
-      <c r="AZ39" s="51"/>
-    </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ39" s="53"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
         <v>79</v>
       </c>
@@ -3607,13 +3607,13 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
-      <c r="AD40" s="48"/>
+      <c r="AD40" s="50"/>
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
-      <c r="AJ40" s="48"/>
+      <c r="AJ40" s="50"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
       <c r="AM40" s="44" t="s">
@@ -3621,19 +3621,19 @@
       </c>
       <c r="AN40" s="2"/>
       <c r="AO40" s="2"/>
-      <c r="AP40" s="48"/>
+      <c r="AP40" s="50"/>
       <c r="AQ40" s="2"/>
       <c r="AR40" s="2"/>
       <c r="AS40" s="2"/>
       <c r="AT40" s="2"/>
       <c r="AU40" s="2"/>
-      <c r="AV40" s="48"/>
+      <c r="AV40" s="50"/>
       <c r="AW40" s="2"/>
       <c r="AX40" s="2"/>
       <c r="AY40" s="2"/>
-      <c r="AZ40" s="51"/>
-    </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ40" s="53"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
         <v>79</v>
       </c>
@@ -3667,13 +3667,13 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
-      <c r="AD41" s="48"/>
+      <c r="AD41" s="50"/>
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
-      <c r="AJ41" s="48"/>
+      <c r="AJ41" s="50"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
       <c r="AM41" s="44" t="s">
@@ -3681,19 +3681,19 @@
       </c>
       <c r="AN41" s="2"/>
       <c r="AO41" s="2"/>
-      <c r="AP41" s="48"/>
+      <c r="AP41" s="50"/>
       <c r="AQ41" s="2"/>
       <c r="AR41" s="2"/>
       <c r="AS41" s="2"/>
       <c r="AT41" s="2"/>
       <c r="AU41" s="2"/>
-      <c r="AV41" s="48"/>
+      <c r="AV41" s="50"/>
       <c r="AW41" s="2"/>
       <c r="AX41" s="2"/>
       <c r="AY41" s="2"/>
-      <c r="AZ41" s="51"/>
-    </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ41" s="53"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
         <v>79</v>
       </c>
@@ -3727,13 +3727,13 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-      <c r="AD42" s="48"/>
+      <c r="AD42" s="50"/>
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2"/>
-      <c r="AJ42" s="48"/>
+      <c r="AJ42" s="50"/>
       <c r="AK42" s="2"/>
       <c r="AL42" s="2"/>
       <c r="AM42" s="2"/>
@@ -3741,19 +3741,19 @@
         <v>106</v>
       </c>
       <c r="AO42" s="2"/>
-      <c r="AP42" s="48"/>
+      <c r="AP42" s="50"/>
       <c r="AQ42" s="2"/>
       <c r="AR42" s="2"/>
       <c r="AS42" s="2"/>
       <c r="AT42" s="2"/>
       <c r="AU42" s="2"/>
-      <c r="AV42" s="48"/>
+      <c r="AV42" s="50"/>
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
       <c r="AY42" s="2"/>
-      <c r="AZ42" s="51"/>
-    </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ42" s="53"/>
+    </row>
+    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
         <v>79</v>
       </c>
@@ -3787,13 +3787,13 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
-      <c r="AD43" s="48"/>
+      <c r="AD43" s="50"/>
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="2"/>
-      <c r="AJ43" s="48"/>
+      <c r="AJ43" s="50"/>
       <c r="AK43" s="2"/>
       <c r="AL43" s="2"/>
       <c r="AM43" s="2"/>
@@ -3801,19 +3801,19 @@
         <v>106</v>
       </c>
       <c r="AO43" s="2"/>
-      <c r="AP43" s="48"/>
+      <c r="AP43" s="50"/>
       <c r="AQ43" s="2"/>
       <c r="AR43" s="2"/>
       <c r="AS43" s="2"/>
       <c r="AT43" s="2"/>
       <c r="AU43" s="2"/>
-      <c r="AV43" s="48"/>
+      <c r="AV43" s="50"/>
       <c r="AW43" s="2"/>
       <c r="AX43" s="2"/>
       <c r="AY43" s="2"/>
-      <c r="AZ43" s="51"/>
-    </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ43" s="53"/>
+    </row>
+    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
         <v>87</v>
       </c>
@@ -3845,31 +3845,31 @@
       <c r="AA44" s="28"/>
       <c r="AB44" s="28"/>
       <c r="AC44" s="28"/>
-      <c r="AD44" s="48"/>
+      <c r="AD44" s="50"/>
       <c r="AE44" s="28"/>
       <c r="AF44" s="28"/>
       <c r="AG44" s="28"/>
       <c r="AH44" s="28"/>
       <c r="AI44" s="28"/>
-      <c r="AJ44" s="48"/>
+      <c r="AJ44" s="50"/>
       <c r="AK44" s="28"/>
       <c r="AL44" s="28"/>
       <c r="AM44" s="28"/>
       <c r="AN44" s="28"/>
       <c r="AO44" s="28"/>
-      <c r="AP44" s="48"/>
+      <c r="AP44" s="50"/>
       <c r="AQ44" s="28"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="28"/>
       <c r="AT44" s="28"/>
       <c r="AU44" s="28"/>
-      <c r="AV44" s="48"/>
+      <c r="AV44" s="50"/>
       <c r="AW44" s="28"/>
       <c r="AX44" s="28"/>
       <c r="AY44" s="28"/>
-      <c r="AZ44" s="51"/>
-    </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ44" s="53"/>
+    </row>
+    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
         <v>91</v>
       </c>
@@ -3903,13 +3903,13 @@
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
-      <c r="AD45" s="48"/>
+      <c r="AD45" s="50"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
-      <c r="AJ45" s="48"/>
+      <c r="AJ45" s="50"/>
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
@@ -3917,7 +3917,7 @@
       <c r="AO45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AP45" s="48"/>
+      <c r="AP45" s="50"/>
       <c r="AQ45" s="44" t="s">
         <v>106</v>
       </c>
@@ -3933,7 +3933,7 @@
       <c r="AU45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AV45" s="48"/>
+      <c r="AV45" s="50"/>
       <c r="AW45" s="44" t="s">
         <v>106</v>
       </c>
@@ -3943,9 +3943,9 @@
       <c r="AY45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ45" s="51"/>
-    </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ45" s="53"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
         <v>91</v>
       </c>
@@ -3977,31 +3977,31 @@
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
-      <c r="AD46" s="48"/>
+      <c r="AD46" s="50"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
-      <c r="AJ46" s="48"/>
+      <c r="AJ46" s="50"/>
       <c r="AK46" s="3"/>
       <c r="AL46" s="3"/>
       <c r="AM46" s="3"/>
       <c r="AN46" s="3"/>
       <c r="AO46" s="3"/>
-      <c r="AP46" s="48"/>
+      <c r="AP46" s="50"/>
       <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
       <c r="AT46" s="3"/>
       <c r="AU46" s="3"/>
-      <c r="AV46" s="48"/>
+      <c r="AV46" s="50"/>
       <c r="AW46" s="3"/>
       <c r="AX46" s="3"/>
       <c r="AY46" s="3"/>
-      <c r="AZ46" s="51"/>
-    </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ46" s="53"/>
+    </row>
+    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
         <v>91</v>
       </c>
@@ -4033,31 +4033,31 @@
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
-      <c r="AD47" s="48"/>
+      <c r="AD47" s="50"/>
       <c r="AE47" s="3"/>
       <c r="AF47" s="3"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
-      <c r="AJ47" s="48"/>
+      <c r="AJ47" s="50"/>
       <c r="AK47" s="3"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="3"/>
       <c r="AN47" s="3"/>
       <c r="AO47" s="3"/>
-      <c r="AP47" s="48"/>
+      <c r="AP47" s="50"/>
       <c r="AQ47" s="3"/>
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
       <c r="AU47" s="3"/>
-      <c r="AV47" s="48"/>
+      <c r="AV47" s="50"/>
       <c r="AW47" s="3"/>
       <c r="AX47" s="3"/>
       <c r="AY47" s="3"/>
-      <c r="AZ47" s="51"/>
-    </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ47" s="53"/>
+    </row>
+    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
         <v>91</v>
       </c>
@@ -4091,19 +4091,19 @@
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
-      <c r="AD48" s="48"/>
+      <c r="AD48" s="50"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
-      <c r="AJ48" s="48"/>
+      <c r="AJ48" s="50"/>
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
       <c r="AO48" s="3"/>
-      <c r="AP48" s="48"/>
+      <c r="AP48" s="50"/>
       <c r="AQ48" s="44" t="s">
         <v>106</v>
       </c>
@@ -4119,7 +4119,7 @@
       <c r="AU48" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AV48" s="48"/>
+      <c r="AV48" s="50"/>
       <c r="AW48" s="44" t="s">
         <v>106</v>
       </c>
@@ -4129,9 +4129,9 @@
       <c r="AY48" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ48" s="51"/>
-    </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ48" s="53"/>
+    </row>
+    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="s">
         <v>91</v>
       </c>
@@ -4163,31 +4163,31 @@
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
-      <c r="AD49" s="48"/>
+      <c r="AD49" s="50"/>
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
-      <c r="AJ49" s="48"/>
+      <c r="AJ49" s="50"/>
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
       <c r="AO49" s="3"/>
-      <c r="AP49" s="48"/>
+      <c r="AP49" s="50"/>
       <c r="AQ49" s="3"/>
       <c r="AR49" s="3"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
-      <c r="AV49" s="48"/>
+      <c r="AV49" s="50"/>
       <c r="AW49" s="3"/>
       <c r="AX49" s="3"/>
       <c r="AY49" s="3"/>
-      <c r="AZ49" s="51"/>
-    </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="AZ49" s="53"/>
+    </row>
+    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
         <v>91</v>
       </c>
@@ -4219,31 +4219,31 @@
       <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
-      <c r="AD50" s="48"/>
+      <c r="AD50" s="50"/>
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
       <c r="AG50" s="3"/>
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
-      <c r="AJ50" s="48"/>
+      <c r="AJ50" s="50"/>
       <c r="AK50" s="3"/>
       <c r="AL50" s="3"/>
       <c r="AM50" s="3"/>
       <c r="AN50" s="3"/>
       <c r="AO50" s="3"/>
-      <c r="AP50" s="48"/>
+      <c r="AP50" s="50"/>
       <c r="AQ50" s="3"/>
       <c r="AR50" s="3"/>
       <c r="AS50" s="3"/>
       <c r="AT50" s="3"/>
       <c r="AU50" s="3"/>
-      <c r="AV50" s="48"/>
+      <c r="AV50" s="50"/>
       <c r="AW50" s="3"/>
       <c r="AX50" s="3"/>
       <c r="AY50" s="3"/>
-      <c r="AZ50" s="51"/>
-    </row>
-    <row r="51" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ50" s="53"/>
+    </row>
+    <row r="51" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="41" t="s">
         <v>91</v>
       </c>
@@ -4277,19 +4277,19 @@
       <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
-      <c r="AD51" s="49"/>
+      <c r="AD51" s="51"/>
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
       <c r="AG51" s="3"/>
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
-      <c r="AJ51" s="49"/>
+      <c r="AJ51" s="51"/>
       <c r="AK51" s="3"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="3"/>
       <c r="AN51" s="3"/>
       <c r="AO51" s="3"/>
-      <c r="AP51" s="49"/>
+      <c r="AP51" s="51"/>
       <c r="AQ51" s="44" t="s">
         <v>106</v>
       </c>
@@ -4305,7 +4305,7 @@
       <c r="AU51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AV51" s="49"/>
+      <c r="AV51" s="51"/>
       <c r="AW51" s="44" t="s">
         <v>106</v>
       </c>
@@ -4315,17 +4315,17 @@
       <c r="AY51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ51" s="52"/>
-    </row>
-    <row r="52" spans="1:52" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="AZ51" s="54"/>
+    </row>
+    <row r="52" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AZ4:AZ51"/>
     <mergeCell ref="U2:Z2"/>
     <mergeCell ref="AD4:AD51"/>
     <mergeCell ref="AJ4:AJ51"/>
     <mergeCell ref="AP4:AP51"/>
     <mergeCell ref="AV4:AV51"/>
-    <mergeCell ref="AZ4:AZ51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
code + gantt-chart update
</commit_message>
<xml_diff>
--- a/Dokumente/Planen/00_Projektablauf_Gantt.xlsx
+++ b/Dokumente/Planen/00_Projektablauf_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvesj\source\ims.project.terminalchat\Dokumente\Planen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75BA71-AB1F-417A-B421-6EC5EA778A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43624B79-A713-4F3A-848A-3C301F092931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27795" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="108">
   <si>
     <t>IPERKA</t>
   </si>
@@ -773,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -894,6 +894,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -906,14 +915,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AP4" sqref="AP4:AP51"/>
+    <sheetView tabSelected="1" zoomScale="36" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AP52" sqref="AP52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,17 +1234,17 @@
       <c r="N2" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="O2" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="U2" s="48" t="s">
+      <c r="U2" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
     </row>
     <row r="3" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38" t="s">
@@ -1373,19 +1376,19 @@
       <c r="AQ3" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AR3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AS3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AT3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AU3" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AV3" s="30" t="s">
         <v>48</v>
       </c>
       <c r="AW3" s="8" t="s">
@@ -1433,29 +1436,29 @@
       <c r="AA4" s="20"/>
       <c r="AB4" s="20"/>
       <c r="AC4" s="20"/>
-      <c r="AD4" s="49"/>
+      <c r="AD4" s="52"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="20"/>
       <c r="AG4" s="20"/>
       <c r="AH4" s="20"/>
       <c r="AI4" s="20"/>
-      <c r="AJ4" s="49"/>
+      <c r="AJ4" s="52"/>
       <c r="AK4" s="20"/>
       <c r="AL4" s="20"/>
       <c r="AM4" s="20"/>
       <c r="AN4" s="20"/>
       <c r="AO4" s="20"/>
-      <c r="AP4" s="49"/>
+      <c r="AP4" s="52"/>
       <c r="AQ4" s="20"/>
       <c r="AR4" s="20"/>
       <c r="AS4" s="20"/>
       <c r="AT4" s="20"/>
       <c r="AU4" s="20"/>
-      <c r="AV4" s="49"/>
+      <c r="AV4" s="52"/>
       <c r="AW4" s="20"/>
       <c r="AX4" s="20"/>
       <c r="AY4" s="20"/>
-      <c r="AZ4" s="52" t="s">
+      <c r="AZ4" s="48" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1497,29 +1500,29 @@
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="50"/>
+      <c r="AD5" s="53"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
-      <c r="AJ5" s="50"/>
+      <c r="AJ5" s="53"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="2"/>
       <c r="AM5" s="2"/>
       <c r="AN5" s="2"/>
       <c r="AO5" s="2"/>
-      <c r="AP5" s="50"/>
+      <c r="AP5" s="53"/>
       <c r="AQ5" s="2"/>
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
-      <c r="AV5" s="50"/>
+      <c r="AV5" s="53"/>
       <c r="AW5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AY5" s="2"/>
-      <c r="AZ5" s="53"/>
+      <c r="AZ5" s="49"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -1557,29 +1560,29 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
-      <c r="AD6" s="50"/>
+      <c r="AD6" s="53"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
-      <c r="AJ6" s="50"/>
+      <c r="AJ6" s="53"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
-      <c r="AP6" s="50"/>
+      <c r="AP6" s="53"/>
       <c r="AQ6" s="2"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="2"/>
       <c r="AU6" s="2"/>
-      <c r="AV6" s="50"/>
+      <c r="AV6" s="53"/>
       <c r="AW6" s="2"/>
       <c r="AX6" s="2"/>
       <c r="AY6" s="2"/>
-      <c r="AZ6" s="53"/>
+      <c r="AZ6" s="49"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
@@ -1617,29 +1620,29 @@
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="50"/>
+      <c r="AD7" s="53"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
-      <c r="AJ7" s="50"/>
+      <c r="AJ7" s="53"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
-      <c r="AP7" s="50"/>
+      <c r="AP7" s="53"/>
       <c r="AQ7" s="2"/>
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="2"/>
       <c r="AU7" s="2"/>
-      <c r="AV7" s="50"/>
+      <c r="AV7" s="53"/>
       <c r="AW7" s="2"/>
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
-      <c r="AZ7" s="53"/>
+      <c r="AZ7" s="49"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
@@ -1677,29 +1680,29 @@
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="50"/>
+      <c r="AD8" s="53"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
-      <c r="AJ8" s="50"/>
+      <c r="AJ8" s="53"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
-      <c r="AP8" s="50"/>
+      <c r="AP8" s="53"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="2"/>
       <c r="AU8" s="2"/>
-      <c r="AV8" s="50"/>
+      <c r="AV8" s="53"/>
       <c r="AW8" s="2"/>
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
-      <c r="AZ8" s="53"/>
+      <c r="AZ8" s="49"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
@@ -1737,29 +1740,29 @@
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="50"/>
+      <c r="AD9" s="53"/>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
-      <c r="AJ9" s="50"/>
+      <c r="AJ9" s="53"/>
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
-      <c r="AP9" s="50"/>
+      <c r="AP9" s="53"/>
       <c r="AQ9" s="2"/>
       <c r="AR9" s="2"/>
       <c r="AS9" s="2"/>
       <c r="AT9" s="2"/>
       <c r="AU9" s="2"/>
-      <c r="AV9" s="50"/>
+      <c r="AV9" s="53"/>
       <c r="AW9" s="2"/>
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
-      <c r="AZ9" s="53"/>
+      <c r="AZ9" s="49"/>
     </row>
     <row r="10" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
@@ -1799,29 +1802,29 @@
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="50"/>
+      <c r="AD10" s="53"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
-      <c r="AJ10" s="50"/>
+      <c r="AJ10" s="53"/>
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
-      <c r="AP10" s="50"/>
+      <c r="AP10" s="53"/>
       <c r="AQ10" s="2"/>
       <c r="AR10" s="2"/>
       <c r="AS10" s="2"/>
       <c r="AT10" s="2"/>
       <c r="AU10" s="2"/>
-      <c r="AV10" s="50"/>
+      <c r="AV10" s="53"/>
       <c r="AW10" s="2"/>
       <c r="AX10" s="2"/>
       <c r="AY10" s="2"/>
-      <c r="AZ10" s="53"/>
+      <c r="AZ10" s="49"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -1859,29 +1862,29 @@
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="50"/>
+      <c r="AD11" s="53"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
-      <c r="AJ11" s="50"/>
+      <c r="AJ11" s="53"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
-      <c r="AP11" s="50"/>
+      <c r="AP11" s="53"/>
       <c r="AQ11" s="2"/>
       <c r="AR11" s="2"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="2"/>
       <c r="AU11" s="2"/>
-      <c r="AV11" s="50"/>
+      <c r="AV11" s="53"/>
       <c r="AW11" s="2"/>
       <c r="AX11" s="2"/>
       <c r="AY11" s="2"/>
-      <c r="AZ11" s="53"/>
+      <c r="AZ11" s="49"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
@@ -1919,29 +1922,29 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="50"/>
+      <c r="AD12" s="53"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="50"/>
+      <c r="AJ12" s="53"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
-      <c r="AP12" s="50"/>
+      <c r="AP12" s="53"/>
       <c r="AQ12" s="2"/>
       <c r="AR12" s="2"/>
       <c r="AS12" s="2"/>
       <c r="AT12" s="2"/>
       <c r="AU12" s="2"/>
-      <c r="AV12" s="50"/>
+      <c r="AV12" s="53"/>
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
-      <c r="AZ12" s="53"/>
+      <c r="AZ12" s="49"/>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
@@ -1979,29 +1982,29 @@
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="50"/>
+      <c r="AD13" s="53"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="50"/>
+      <c r="AJ13" s="53"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
-      <c r="AP13" s="50"/>
+      <c r="AP13" s="53"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
       <c r="AS13" s="2"/>
       <c r="AT13" s="2"/>
       <c r="AU13" s="2"/>
-      <c r="AV13" s="50"/>
+      <c r="AV13" s="53"/>
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
-      <c r="AZ13" s="53"/>
+      <c r="AZ13" s="49"/>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
@@ -2039,29 +2042,29 @@
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="50"/>
+      <c r="AD14" s="53"/>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
-      <c r="AJ14" s="50"/>
+      <c r="AJ14" s="53"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
-      <c r="AP14" s="50"/>
+      <c r="AP14" s="53"/>
       <c r="AQ14" s="2"/>
       <c r="AR14" s="2"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="2"/>
       <c r="AU14" s="2"/>
-      <c r="AV14" s="50"/>
+      <c r="AV14" s="53"/>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
-      <c r="AZ14" s="53"/>
+      <c r="AZ14" s="49"/>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
@@ -2099,29 +2102,29 @@
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="50"/>
+      <c r="AD15" s="53"/>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
-      <c r="AJ15" s="50"/>
+      <c r="AJ15" s="53"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
-      <c r="AP15" s="50"/>
+      <c r="AP15" s="53"/>
       <c r="AQ15" s="2"/>
       <c r="AR15" s="2"/>
       <c r="AS15" s="2"/>
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
-      <c r="AV15" s="50"/>
+      <c r="AV15" s="53"/>
       <c r="AW15" s="2"/>
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
-      <c r="AZ15" s="53"/>
+      <c r="AZ15" s="49"/>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
@@ -2157,29 +2160,29 @@
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="50"/>
+      <c r="AD16" s="53"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
-      <c r="AJ16" s="50"/>
+      <c r="AJ16" s="53"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="50"/>
+      <c r="AP16" s="53"/>
       <c r="AQ16" s="2"/>
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="2"/>
       <c r="AU16" s="2"/>
-      <c r="AV16" s="50"/>
+      <c r="AV16" s="53"/>
       <c r="AW16" s="2"/>
       <c r="AX16" s="2"/>
       <c r="AY16" s="2"/>
-      <c r="AZ16" s="53"/>
+      <c r="AZ16" s="49"/>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
@@ -2217,29 +2220,29 @@
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="50"/>
+      <c r="AD17" s="53"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
-      <c r="AJ17" s="50"/>
+      <c r="AJ17" s="53"/>
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="50"/>
+      <c r="AP17" s="53"/>
       <c r="AQ17" s="2"/>
       <c r="AR17" s="2"/>
       <c r="AS17" s="2"/>
       <c r="AT17" s="2"/>
       <c r="AU17" s="2"/>
-      <c r="AV17" s="50"/>
+      <c r="AV17" s="53"/>
       <c r="AW17" s="2"/>
       <c r="AX17" s="2"/>
       <c r="AY17" s="2"/>
-      <c r="AZ17" s="53"/>
+      <c r="AZ17" s="49"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
@@ -2277,29 +2280,29 @@
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
-      <c r="AD18" s="50"/>
+      <c r="AD18" s="53"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
-      <c r="AJ18" s="50"/>
+      <c r="AJ18" s="53"/>
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
-      <c r="AP18" s="50"/>
+      <c r="AP18" s="53"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="2"/>
       <c r="AS18" s="2"/>
       <c r="AT18" s="2"/>
       <c r="AU18" s="2"/>
-      <c r="AV18" s="50"/>
+      <c r="AV18" s="53"/>
       <c r="AW18" s="2"/>
       <c r="AX18" s="2"/>
       <c r="AY18" s="2"/>
-      <c r="AZ18" s="53"/>
+      <c r="AZ18" s="49"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
@@ -2343,29 +2346,29 @@
       <c r="AC19" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="AD19" s="50"/>
+      <c r="AD19" s="53"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
-      <c r="AJ19" s="50"/>
+      <c r="AJ19" s="53"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
-      <c r="AP19" s="50"/>
+      <c r="AP19" s="53"/>
       <c r="AQ19" s="2"/>
       <c r="AR19" s="2"/>
       <c r="AS19" s="2"/>
       <c r="AT19" s="2"/>
       <c r="AU19" s="2"/>
-      <c r="AV19" s="50"/>
+      <c r="AV19" s="53"/>
       <c r="AW19" s="2"/>
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
-      <c r="AZ19" s="53"/>
+      <c r="AZ19" s="49"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
@@ -2399,29 +2402,29 @@
       <c r="AA20" s="24"/>
       <c r="AB20" s="24"/>
       <c r="AC20" s="24"/>
-      <c r="AD20" s="50"/>
+      <c r="AD20" s="53"/>
       <c r="AE20" s="24"/>
       <c r="AF20" s="24"/>
       <c r="AG20" s="24"/>
       <c r="AH20" s="24"/>
       <c r="AI20" s="24"/>
-      <c r="AJ20" s="50"/>
+      <c r="AJ20" s="53"/>
       <c r="AK20" s="24"/>
       <c r="AL20" s="24"/>
       <c r="AM20" s="24"/>
       <c r="AN20" s="24"/>
       <c r="AO20" s="24"/>
-      <c r="AP20" s="50"/>
+      <c r="AP20" s="53"/>
       <c r="AQ20" s="24"/>
       <c r="AR20" s="24"/>
       <c r="AS20" s="24"/>
       <c r="AT20" s="24"/>
       <c r="AU20" s="24"/>
-      <c r="AV20" s="50"/>
+      <c r="AV20" s="53"/>
       <c r="AW20" s="24"/>
       <c r="AX20" s="24"/>
       <c r="AY20" s="24"/>
-      <c r="AZ20" s="53"/>
+      <c r="AZ20" s="49"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
@@ -2457,29 +2460,29 @@
       <c r="AA21" s="2"/>
       <c r="AB21" s="47"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="50"/>
+      <c r="AD21" s="53"/>
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="50"/>
+      <c r="AJ21" s="53"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
-      <c r="AP21" s="50"/>
+      <c r="AP21" s="53"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
       <c r="AS21" s="2"/>
       <c r="AT21" s="2"/>
       <c r="AU21" s="2"/>
-      <c r="AV21" s="50"/>
+      <c r="AV21" s="53"/>
       <c r="AW21" s="2"/>
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
-      <c r="AZ21" s="53"/>
+      <c r="AZ21" s="49"/>
     </row>
     <row r="22" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
@@ -2519,31 +2522,31 @@
         <v>105</v>
       </c>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="50"/>
-      <c r="AE22" s="44" t="s">
+      <c r="AD22" s="53"/>
+      <c r="AE22" s="43" t="s">
         <v>106</v>
       </c>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
-      <c r="AJ22" s="50"/>
+      <c r="AJ22" s="53"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
-      <c r="AP22" s="50"/>
+      <c r="AP22" s="53"/>
       <c r="AQ22" s="2"/>
       <c r="AR22" s="2"/>
       <c r="AS22" s="2"/>
       <c r="AT22" s="2"/>
       <c r="AU22" s="2"/>
-      <c r="AV22" s="50"/>
+      <c r="AV22" s="53"/>
       <c r="AW22" s="2"/>
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
-      <c r="AZ22" s="53"/>
+      <c r="AZ22" s="49"/>
     </row>
     <row r="23" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
@@ -2581,31 +2584,33 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="50"/>
+      <c r="AD23" s="53"/>
       <c r="AE23" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AF23" s="2"/>
+      <c r="AF23" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="50"/>
+      <c r="AJ23" s="53"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="50"/>
+      <c r="AP23" s="53"/>
       <c r="AQ23" s="2"/>
       <c r="AR23" s="2"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="2"/>
       <c r="AU23" s="2"/>
-      <c r="AV23" s="50"/>
+      <c r="AV23" s="53"/>
       <c r="AW23" s="2"/>
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
-      <c r="AZ23" s="53"/>
+      <c r="AZ23" s="49"/>
     </row>
     <row r="24" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
@@ -2643,31 +2648,39 @@
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="50"/>
+      <c r="AD24" s="53"/>
       <c r="AE24" s="2"/>
       <c r="AF24" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AG24" s="2"/>
+      <c r="AG24" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-      <c r="AJ24" s="50"/>
+      <c r="AJ24" s="53"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
-      <c r="AP24" s="50"/>
+      <c r="AP24" s="53"/>
       <c r="AQ24" s="2"/>
       <c r="AR24" s="2"/>
       <c r="AS24" s="2"/>
       <c r="AT24" s="2"/>
       <c r="AU24" s="2"/>
-      <c r="AV24" s="50"/>
-      <c r="AW24" s="2"/>
-      <c r="AX24" s="2"/>
-      <c r="AY24" s="2"/>
-      <c r="AZ24" s="53"/>
+      <c r="AV24" s="53"/>
+      <c r="AW24" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX24" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY24" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ24" s="49"/>
     </row>
     <row r="25" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
@@ -2705,31 +2718,33 @@
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="50"/>
+      <c r="AD25" s="53"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="44" t="s">
         <v>106</v>
       </c>
       <c r="AG25" s="2"/>
-      <c r="AH25" s="2"/>
+      <c r="AH25" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="50"/>
+      <c r="AJ25" s="53"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="2"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
-      <c r="AP25" s="50"/>
+      <c r="AP25" s="53"/>
       <c r="AQ25" s="2"/>
       <c r="AR25" s="2"/>
       <c r="AS25" s="2"/>
       <c r="AT25" s="2"/>
       <c r="AU25" s="2"/>
-      <c r="AV25" s="50"/>
+      <c r="AV25" s="53"/>
       <c r="AW25" s="2"/>
       <c r="AX25" s="2"/>
       <c r="AY25" s="2"/>
-      <c r="AZ25" s="53"/>
+      <c r="AZ25" s="49"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
@@ -2765,29 +2780,29 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="50"/>
+      <c r="AD26" s="53"/>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="50"/>
+      <c r="AJ26" s="53"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
-      <c r="AP26" s="50"/>
+      <c r="AP26" s="53"/>
       <c r="AQ26" s="2"/>
       <c r="AR26" s="2"/>
       <c r="AS26" s="2"/>
       <c r="AT26" s="2"/>
       <c r="AU26" s="2"/>
-      <c r="AV26" s="50"/>
+      <c r="AV26" s="53"/>
       <c r="AW26" s="2"/>
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
-      <c r="AZ26" s="53"/>
+      <c r="AZ26" s="49"/>
     </row>
     <row r="27" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
@@ -2825,31 +2840,33 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
-      <c r="AD27" s="50"/>
+      <c r="AD27" s="53"/>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="44" t="s">
         <v>106</v>
       </c>
       <c r="AH27" s="2"/>
-      <c r="AI27" s="2"/>
-      <c r="AJ27" s="50"/>
+      <c r="AI27" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ27" s="53"/>
       <c r="AK27" s="2"/>
       <c r="AL27" s="2"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
-      <c r="AP27" s="50"/>
+      <c r="AP27" s="53"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
       <c r="AS27" s="2"/>
       <c r="AT27" s="2"/>
       <c r="AU27" s="2"/>
-      <c r="AV27" s="50"/>
+      <c r="AV27" s="53"/>
       <c r="AW27" s="2"/>
       <c r="AX27" s="2"/>
       <c r="AY27" s="2"/>
-      <c r="AZ27" s="53"/>
+      <c r="AZ27" s="49"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
@@ -2885,29 +2902,29 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-      <c r="AD28" s="50"/>
+      <c r="AD28" s="53"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-      <c r="AJ28" s="50"/>
+      <c r="AJ28" s="53"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
-      <c r="AP28" s="50"/>
+      <c r="AP28" s="53"/>
       <c r="AQ28" s="2"/>
       <c r="AR28" s="2"/>
       <c r="AS28" s="2"/>
       <c r="AT28" s="2"/>
       <c r="AU28" s="2"/>
-      <c r="AV28" s="50"/>
+      <c r="AV28" s="53"/>
       <c r="AW28" s="2"/>
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
-      <c r="AZ28" s="53"/>
+      <c r="AZ28" s="49"/>
     </row>
     <row r="29" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
@@ -2945,7 +2962,7 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="50"/>
+      <c r="AD29" s="53"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
@@ -2953,23 +2970,33 @@
         <v>106</v>
       </c>
       <c r="AI29" s="2"/>
-      <c r="AJ29" s="50"/>
-      <c r="AK29" s="2"/>
-      <c r="AL29" s="2"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL29" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
-      <c r="AP29" s="50"/>
+      <c r="AP29" s="53"/>
       <c r="AQ29" s="2"/>
       <c r="AR29" s="2"/>
       <c r="AS29" s="2"/>
       <c r="AT29" s="2"/>
       <c r="AU29" s="2"/>
-      <c r="AV29" s="50"/>
-      <c r="AW29" s="2"/>
-      <c r="AX29" s="2"/>
-      <c r="AY29" s="2"/>
-      <c r="AZ29" s="53"/>
+      <c r="AV29" s="53"/>
+      <c r="AW29" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX29" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY29" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ29" s="49"/>
     </row>
     <row r="30" spans="1:52" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
@@ -3007,7 +3034,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-      <c r="AD30" s="50"/>
+      <c r="AD30" s="53"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
@@ -3015,23 +3042,25 @@
         <v>106</v>
       </c>
       <c r="AI30" s="2"/>
-      <c r="AJ30" s="50"/>
+      <c r="AJ30" s="53"/>
       <c r="AK30" s="2"/>
       <c r="AL30" s="2"/>
-      <c r="AM30" s="2"/>
+      <c r="AM30" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
-      <c r="AP30" s="50"/>
+      <c r="AP30" s="53"/>
       <c r="AQ30" s="2"/>
       <c r="AR30" s="2"/>
       <c r="AS30" s="2"/>
       <c r="AT30" s="2"/>
       <c r="AU30" s="2"/>
-      <c r="AV30" s="50"/>
+      <c r="AV30" s="53"/>
       <c r="AW30" s="2"/>
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
-      <c r="AZ30" s="53"/>
+      <c r="AZ30" s="49"/>
     </row>
     <row r="31" spans="1:52" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
@@ -3069,7 +3098,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="50"/>
+      <c r="AD31" s="53"/>
       <c r="AE31" s="2"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
@@ -3077,23 +3106,25 @@
       <c r="AI31" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AJ31" s="50"/>
+      <c r="AJ31" s="53"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="2"/>
-      <c r="AM31" s="2"/>
+      <c r="AM31" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AN31" s="2"/>
       <c r="AO31" s="2"/>
-      <c r="AP31" s="50"/>
+      <c r="AP31" s="53"/>
       <c r="AQ31" s="2"/>
       <c r="AR31" s="2"/>
       <c r="AS31" s="2"/>
       <c r="AT31" s="2"/>
       <c r="AU31" s="2"/>
-      <c r="AV31" s="50"/>
+      <c r="AV31" s="53"/>
       <c r="AW31" s="2"/>
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
-      <c r="AZ31" s="53"/>
+      <c r="AZ31" s="49"/>
     </row>
     <row r="32" spans="1:52" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
@@ -3131,7 +3162,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="50"/>
+      <c r="AD32" s="53"/>
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
@@ -3139,23 +3170,27 @@
       <c r="AI32" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AJ32" s="50"/>
+      <c r="AJ32" s="53"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
       <c r="AM32" s="2"/>
-      <c r="AN32" s="2"/>
-      <c r="AO32" s="2"/>
-      <c r="AP32" s="50"/>
+      <c r="AN32" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AO32" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP32" s="53"/>
       <c r="AQ32" s="2"/>
       <c r="AR32" s="2"/>
       <c r="AS32" s="2"/>
       <c r="AT32" s="2"/>
       <c r="AU32" s="2"/>
-      <c r="AV32" s="50"/>
+      <c r="AV32" s="53"/>
       <c r="AW32" s="2"/>
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
-      <c r="AZ32" s="53"/>
+      <c r="AZ32" s="49"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
@@ -3189,29 +3224,29 @@
       <c r="AA33" s="24"/>
       <c r="AB33" s="24"/>
       <c r="AC33" s="24"/>
-      <c r="AD33" s="50"/>
+      <c r="AD33" s="53"/>
       <c r="AE33" s="24"/>
       <c r="AF33" s="24"/>
       <c r="AG33" s="24"/>
       <c r="AH33" s="24"/>
       <c r="AI33" s="24"/>
-      <c r="AJ33" s="50"/>
+      <c r="AJ33" s="53"/>
       <c r="AK33" s="24"/>
       <c r="AL33" s="24"/>
       <c r="AM33" s="24"/>
       <c r="AN33" s="24"/>
       <c r="AO33" s="24"/>
-      <c r="AP33" s="50"/>
+      <c r="AP33" s="53"/>
       <c r="AQ33" s="24"/>
       <c r="AR33" s="24"/>
       <c r="AS33" s="24"/>
       <c r="AT33" s="24"/>
       <c r="AU33" s="24"/>
-      <c r="AV33" s="50"/>
+      <c r="AV33" s="53"/>
       <c r="AW33" s="24"/>
       <c r="AX33" s="24"/>
       <c r="AY33" s="24"/>
-      <c r="AZ33" s="53"/>
+      <c r="AZ33" s="49"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
@@ -3247,13 +3282,13 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="50"/>
+      <c r="AD34" s="53"/>
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="50"/>
+      <c r="AJ34" s="53"/>
       <c r="AK34" s="44" t="s">
         <v>106</v>
       </c>
@@ -3261,17 +3296,19 @@
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2"/>
-      <c r="AP34" s="50"/>
-      <c r="AQ34" s="2"/>
+      <c r="AP34" s="53"/>
+      <c r="AQ34" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR34" s="2"/>
       <c r="AS34" s="2"/>
       <c r="AT34" s="2"/>
       <c r="AU34" s="2"/>
-      <c r="AV34" s="50"/>
+      <c r="AV34" s="53"/>
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
       <c r="AY34" s="2"/>
-      <c r="AZ34" s="53"/>
+      <c r="AZ34" s="49"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
@@ -3307,13 +3344,13 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
-      <c r="AD35" s="50"/>
+      <c r="AD35" s="53"/>
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-      <c r="AJ35" s="50"/>
+      <c r="AJ35" s="53"/>
       <c r="AK35" s="44" t="s">
         <v>106</v>
       </c>
@@ -3321,17 +3358,19 @@
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
       <c r="AO35" s="2"/>
-      <c r="AP35" s="50"/>
-      <c r="AQ35" s="2"/>
+      <c r="AP35" s="53"/>
+      <c r="AQ35" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR35" s="2"/>
       <c r="AS35" s="2"/>
       <c r="AT35" s="2"/>
       <c r="AU35" s="2"/>
-      <c r="AV35" s="50"/>
+      <c r="AV35" s="53"/>
       <c r="AW35" s="2"/>
       <c r="AX35" s="2"/>
       <c r="AY35" s="2"/>
-      <c r="AZ35" s="53"/>
+      <c r="AZ35" s="49"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
@@ -3367,13 +3406,13 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
-      <c r="AD36" s="50"/>
+      <c r="AD36" s="53"/>
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-      <c r="AJ36" s="50"/>
+      <c r="AJ36" s="53"/>
       <c r="AK36" s="44" t="s">
         <v>106</v>
       </c>
@@ -3381,17 +3420,19 @@
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
-      <c r="AP36" s="50"/>
-      <c r="AQ36" s="2"/>
+      <c r="AP36" s="53"/>
+      <c r="AQ36" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR36" s="2"/>
       <c r="AS36" s="2"/>
       <c r="AT36" s="2"/>
       <c r="AU36" s="2"/>
-      <c r="AV36" s="50"/>
+      <c r="AV36" s="53"/>
       <c r="AW36" s="2"/>
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
-      <c r="AZ36" s="53"/>
+      <c r="AZ36" s="49"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
@@ -3427,13 +3468,13 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
-      <c r="AD37" s="50"/>
+      <c r="AD37" s="53"/>
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-      <c r="AJ37" s="50"/>
+      <c r="AJ37" s="53"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="44" t="s">
         <v>106</v>
@@ -3441,17 +3482,19 @@
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
-      <c r="AP37" s="50"/>
-      <c r="AQ37" s="2"/>
+      <c r="AP37" s="53"/>
+      <c r="AQ37" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR37" s="2"/>
       <c r="AS37" s="2"/>
       <c r="AT37" s="2"/>
       <c r="AU37" s="2"/>
-      <c r="AV37" s="50"/>
+      <c r="AV37" s="53"/>
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
-      <c r="AZ37" s="53"/>
+      <c r="AZ37" s="49"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
@@ -3487,13 +3530,13 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
-      <c r="AD38" s="50"/>
+      <c r="AD38" s="53"/>
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="2"/>
-      <c r="AJ38" s="50"/>
+      <c r="AJ38" s="53"/>
       <c r="AK38" s="2"/>
       <c r="AL38" s="44" t="s">
         <v>106</v>
@@ -3501,17 +3544,19 @@
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
       <c r="AO38" s="2"/>
-      <c r="AP38" s="50"/>
-      <c r="AQ38" s="2"/>
+      <c r="AP38" s="53"/>
+      <c r="AQ38" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR38" s="2"/>
       <c r="AS38" s="2"/>
       <c r="AT38" s="2"/>
       <c r="AU38" s="2"/>
-      <c r="AV38" s="50"/>
+      <c r="AV38" s="53"/>
       <c r="AW38" s="2"/>
       <c r="AX38" s="2"/>
       <c r="AY38" s="2"/>
-      <c r="AZ38" s="53"/>
+      <c r="AZ38" s="49"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
@@ -3547,13 +3592,13 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
-      <c r="AD39" s="50"/>
+      <c r="AD39" s="53"/>
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
-      <c r="AJ39" s="50"/>
+      <c r="AJ39" s="53"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="2"/>
       <c r="AM39" s="44" t="s">
@@ -3561,17 +3606,19 @@
       </c>
       <c r="AN39" s="2"/>
       <c r="AO39" s="2"/>
-      <c r="AP39" s="50"/>
-      <c r="AQ39" s="2"/>
+      <c r="AP39" s="53"/>
+      <c r="AQ39" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR39" s="2"/>
       <c r="AS39" s="2"/>
       <c r="AT39" s="2"/>
       <c r="AU39" s="2"/>
-      <c r="AV39" s="50"/>
+      <c r="AV39" s="53"/>
       <c r="AW39" s="2"/>
       <c r="AX39" s="2"/>
       <c r="AY39" s="2"/>
-      <c r="AZ39" s="53"/>
+      <c r="AZ39" s="49"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
@@ -3607,13 +3654,13 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
-      <c r="AD40" s="50"/>
+      <c r="AD40" s="53"/>
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
       <c r="AI40" s="2"/>
-      <c r="AJ40" s="50"/>
+      <c r="AJ40" s="53"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
       <c r="AM40" s="44" t="s">
@@ -3621,17 +3668,19 @@
       </c>
       <c r="AN40" s="2"/>
       <c r="AO40" s="2"/>
-      <c r="AP40" s="50"/>
-      <c r="AQ40" s="2"/>
+      <c r="AP40" s="53"/>
+      <c r="AQ40" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR40" s="2"/>
       <c r="AS40" s="2"/>
       <c r="AT40" s="2"/>
       <c r="AU40" s="2"/>
-      <c r="AV40" s="50"/>
+      <c r="AV40" s="53"/>
       <c r="AW40" s="2"/>
       <c r="AX40" s="2"/>
       <c r="AY40" s="2"/>
-      <c r="AZ40" s="53"/>
+      <c r="AZ40" s="49"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
@@ -3667,13 +3716,13 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
-      <c r="AD41" s="50"/>
+      <c r="AD41" s="53"/>
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
-      <c r="AJ41" s="50"/>
+      <c r="AJ41" s="53"/>
       <c r="AK41" s="2"/>
       <c r="AL41" s="2"/>
       <c r="AM41" s="44" t="s">
@@ -3681,17 +3730,19 @@
       </c>
       <c r="AN41" s="2"/>
       <c r="AO41" s="2"/>
-      <c r="AP41" s="50"/>
-      <c r="AQ41" s="2"/>
+      <c r="AP41" s="53"/>
+      <c r="AQ41" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR41" s="2"/>
       <c r="AS41" s="2"/>
       <c r="AT41" s="2"/>
       <c r="AU41" s="2"/>
-      <c r="AV41" s="50"/>
+      <c r="AV41" s="53"/>
       <c r="AW41" s="2"/>
       <c r="AX41" s="2"/>
       <c r="AY41" s="2"/>
-      <c r="AZ41" s="53"/>
+      <c r="AZ41" s="49"/>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
@@ -3727,13 +3778,13 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-      <c r="AD42" s="50"/>
+      <c r="AD42" s="53"/>
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2"/>
-      <c r="AJ42" s="50"/>
+      <c r="AJ42" s="53"/>
       <c r="AK42" s="2"/>
       <c r="AL42" s="2"/>
       <c r="AM42" s="2"/>
@@ -3741,17 +3792,19 @@
         <v>106</v>
       </c>
       <c r="AO42" s="2"/>
-      <c r="AP42" s="50"/>
-      <c r="AQ42" s="2"/>
+      <c r="AP42" s="53"/>
+      <c r="AQ42" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR42" s="2"/>
       <c r="AS42" s="2"/>
       <c r="AT42" s="2"/>
       <c r="AU42" s="2"/>
-      <c r="AV42" s="50"/>
+      <c r="AV42" s="53"/>
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
       <c r="AY42" s="2"/>
-      <c r="AZ42" s="53"/>
+      <c r="AZ42" s="49"/>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
@@ -3787,13 +3840,13 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
-      <c r="AD43" s="50"/>
+      <c r="AD43" s="53"/>
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="2"/>
-      <c r="AJ43" s="50"/>
+      <c r="AJ43" s="53"/>
       <c r="AK43" s="2"/>
       <c r="AL43" s="2"/>
       <c r="AM43" s="2"/>
@@ -3801,17 +3854,19 @@
         <v>106</v>
       </c>
       <c r="AO43" s="2"/>
-      <c r="AP43" s="50"/>
-      <c r="AQ43" s="2"/>
+      <c r="AP43" s="53"/>
+      <c r="AQ43" s="46" t="s">
+        <v>105</v>
+      </c>
       <c r="AR43" s="2"/>
       <c r="AS43" s="2"/>
       <c r="AT43" s="2"/>
       <c r="AU43" s="2"/>
-      <c r="AV43" s="50"/>
+      <c r="AV43" s="53"/>
       <c r="AW43" s="2"/>
       <c r="AX43" s="2"/>
       <c r="AY43" s="2"/>
-      <c r="AZ43" s="53"/>
+      <c r="AZ43" s="49"/>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
@@ -3845,29 +3900,29 @@
       <c r="AA44" s="28"/>
       <c r="AB44" s="28"/>
       <c r="AC44" s="28"/>
-      <c r="AD44" s="50"/>
+      <c r="AD44" s="53"/>
       <c r="AE44" s="28"/>
       <c r="AF44" s="28"/>
       <c r="AG44" s="28"/>
       <c r="AH44" s="28"/>
       <c r="AI44" s="28"/>
-      <c r="AJ44" s="50"/>
+      <c r="AJ44" s="53"/>
       <c r="AK44" s="28"/>
       <c r="AL44" s="28"/>
       <c r="AM44" s="28"/>
       <c r="AN44" s="28"/>
       <c r="AO44" s="28"/>
-      <c r="AP44" s="50"/>
+      <c r="AP44" s="53"/>
       <c r="AQ44" s="28"/>
       <c r="AR44" s="28"/>
       <c r="AS44" s="28"/>
       <c r="AT44" s="28"/>
       <c r="AU44" s="28"/>
-      <c r="AV44" s="50"/>
+      <c r="AV44" s="53"/>
       <c r="AW44" s="28"/>
       <c r="AX44" s="28"/>
       <c r="AY44" s="28"/>
-      <c r="AZ44" s="53"/>
+      <c r="AZ44" s="49"/>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
@@ -3903,13 +3958,13 @@
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
-      <c r="AD45" s="50"/>
+      <c r="AD45" s="53"/>
       <c r="AE45" s="3"/>
       <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
-      <c r="AJ45" s="50"/>
+      <c r="AJ45" s="53"/>
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
       <c r="AM45" s="3"/>
@@ -3917,23 +3972,23 @@
       <c r="AO45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AP45" s="50"/>
+      <c r="AP45" s="53"/>
       <c r="AQ45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AR45" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS45" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT45" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU45" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV45" s="50"/>
+      <c r="AR45" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS45" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT45" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU45" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV45" s="53"/>
       <c r="AW45" s="44" t="s">
         <v>106</v>
       </c>
@@ -3943,7 +3998,7 @@
       <c r="AY45" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ45" s="53"/>
+      <c r="AZ45" s="49"/>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
@@ -3977,29 +4032,29 @@
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
-      <c r="AD46" s="50"/>
+      <c r="AD46" s="53"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
-      <c r="AJ46" s="50"/>
+      <c r="AJ46" s="53"/>
       <c r="AK46" s="3"/>
       <c r="AL46" s="3"/>
       <c r="AM46" s="3"/>
       <c r="AN46" s="3"/>
       <c r="AO46" s="3"/>
-      <c r="AP46" s="50"/>
+      <c r="AP46" s="53"/>
       <c r="AQ46" s="3"/>
       <c r="AR46" s="3"/>
       <c r="AS46" s="3"/>
       <c r="AT46" s="3"/>
       <c r="AU46" s="3"/>
-      <c r="AV46" s="50"/>
+      <c r="AV46" s="53"/>
       <c r="AW46" s="3"/>
       <c r="AX46" s="3"/>
       <c r="AY46" s="3"/>
-      <c r="AZ46" s="53"/>
+      <c r="AZ46" s="49"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
@@ -4033,29 +4088,29 @@
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
-      <c r="AD47" s="50"/>
+      <c r="AD47" s="53"/>
       <c r="AE47" s="3"/>
       <c r="AF47" s="3"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
-      <c r="AJ47" s="50"/>
+      <c r="AJ47" s="53"/>
       <c r="AK47" s="3"/>
       <c r="AL47" s="3"/>
       <c r="AM47" s="3"/>
       <c r="AN47" s="3"/>
       <c r="AO47" s="3"/>
-      <c r="AP47" s="50"/>
+      <c r="AP47" s="53"/>
       <c r="AQ47" s="3"/>
       <c r="AR47" s="3"/>
       <c r="AS47" s="3"/>
       <c r="AT47" s="3"/>
       <c r="AU47" s="3"/>
-      <c r="AV47" s="50"/>
+      <c r="AV47" s="53"/>
       <c r="AW47" s="3"/>
       <c r="AX47" s="3"/>
       <c r="AY47" s="3"/>
-      <c r="AZ47" s="53"/>
+      <c r="AZ47" s="49"/>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
@@ -4091,35 +4146,35 @@
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
-      <c r="AD48" s="50"/>
+      <c r="AD48" s="53"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
-      <c r="AJ48" s="50"/>
+      <c r="AJ48" s="53"/>
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
       <c r="AM48" s="3"/>
       <c r="AN48" s="3"/>
       <c r="AO48" s="3"/>
-      <c r="AP48" s="50"/>
+      <c r="AP48" s="53"/>
       <c r="AQ48" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AR48" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS48" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT48" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU48" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV48" s="50"/>
+      <c r="AR48" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS48" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT48" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU48" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV48" s="53"/>
       <c r="AW48" s="44" t="s">
         <v>106</v>
       </c>
@@ -4129,7 +4184,7 @@
       <c r="AY48" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ48" s="53"/>
+      <c r="AZ48" s="49"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="s">
@@ -4163,29 +4218,29 @@
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
-      <c r="AD49" s="50"/>
+      <c r="AD49" s="53"/>
       <c r="AE49" s="3"/>
       <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
-      <c r="AJ49" s="50"/>
+      <c r="AJ49" s="53"/>
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
       <c r="AM49" s="3"/>
       <c r="AN49" s="3"/>
       <c r="AO49" s="3"/>
-      <c r="AP49" s="50"/>
+      <c r="AP49" s="53"/>
       <c r="AQ49" s="3"/>
       <c r="AR49" s="3"/>
       <c r="AS49" s="3"/>
       <c r="AT49" s="3"/>
       <c r="AU49" s="3"/>
-      <c r="AV49" s="50"/>
+      <c r="AV49" s="53"/>
       <c r="AW49" s="3"/>
       <c r="AX49" s="3"/>
       <c r="AY49" s="3"/>
-      <c r="AZ49" s="53"/>
+      <c r="AZ49" s="49"/>
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
@@ -4219,29 +4274,29 @@
       <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
-      <c r="AD50" s="50"/>
+      <c r="AD50" s="53"/>
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
       <c r="AG50" s="3"/>
       <c r="AH50" s="3"/>
       <c r="AI50" s="3"/>
-      <c r="AJ50" s="50"/>
+      <c r="AJ50" s="53"/>
       <c r="AK50" s="3"/>
       <c r="AL50" s="3"/>
       <c r="AM50" s="3"/>
       <c r="AN50" s="3"/>
       <c r="AO50" s="3"/>
-      <c r="AP50" s="50"/>
+      <c r="AP50" s="53"/>
       <c r="AQ50" s="3"/>
       <c r="AR50" s="3"/>
       <c r="AS50" s="3"/>
       <c r="AT50" s="3"/>
       <c r="AU50" s="3"/>
-      <c r="AV50" s="50"/>
+      <c r="AV50" s="53"/>
       <c r="AW50" s="3"/>
       <c r="AX50" s="3"/>
       <c r="AY50" s="3"/>
-      <c r="AZ50" s="53"/>
+      <c r="AZ50" s="49"/>
     </row>
     <row r="51" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="41" t="s">
@@ -4277,35 +4332,35 @@
       <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
-      <c r="AD51" s="51"/>
+      <c r="AD51" s="54"/>
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
       <c r="AG51" s="3"/>
       <c r="AH51" s="3"/>
       <c r="AI51" s="3"/>
-      <c r="AJ51" s="51"/>
+      <c r="AJ51" s="54"/>
       <c r="AK51" s="3"/>
       <c r="AL51" s="3"/>
       <c r="AM51" s="3"/>
       <c r="AN51" s="3"/>
       <c r="AO51" s="3"/>
-      <c r="AP51" s="51"/>
+      <c r="AP51" s="54"/>
       <c r="AQ51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AR51" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS51" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT51" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU51" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV51" s="51"/>
+      <c r="AR51" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS51" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT51" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU51" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV51" s="54"/>
       <c r="AW51" s="44" t="s">
         <v>106</v>
       </c>
@@ -4315,7 +4370,7 @@
       <c r="AY51" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="AZ51" s="54"/>
+      <c r="AZ51" s="50"/>
     </row>
     <row r="52" spans="1:52" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>